<commit_message>
Microsoft Excel INDEX() Function
</commit_message>
<xml_diff>
--- a/Section 25: Working with Excel's Lookup Functions/Resources/Excel103-AdvancedExercises.xlsx
+++ b/Section 25: Working with Excel's Lookup Functions/Resources/Excel103-AdvancedExercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolinecrandell/Documents/Employment/*Applications/2022.12 Job Apps/GitHub/excel/Section 25: Working with Excel's Lookup Functions/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068493CF-E289-2341-8E93-54E8BCF7E418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C743D1A-2376-5E4B-92A4-325F4919A548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16880" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -11488,8 +11488,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="B1:G18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -13005,7 +13005,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -13052,13 +13052,19 @@
       <c r="A6" s="62" t="s">
         <v>228</v>
       </c>
-      <c r="B6" s="57"/>
+      <c r="B6" s="57">
+        <f>HLOOKUP($B$3,'Master Inventory List'!$A$2:$G$5,3,FALSE)</f>
+        <v>110</v>
+      </c>
     </row>
     <row r="7" spans="1:2" ht="14" thickBot="1">
       <c r="A7" s="63" t="s">
         <v>227</v>
       </c>
-      <c r="B7" s="57"/>
+      <c r="B7" s="57">
+        <f>HLOOKUP($B$3,'Master Inventory List'!$A$2:$G$5,4,FALSE)</f>
+        <v>115</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -13186,8 +13192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A99380-3415-42C6-8C41-613698A280FA}">
   <dimension ref="B2:F19"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -13226,7 +13232,10 @@
       <c r="B4" s="68">
         <v>1054</v>
       </c>
-      <c r="C4" s="68"/>
+      <c r="C4" s="68" t="str">
+        <f>INDEX('INDEX MATCH Master Emp List'!$A$1:$I$38,10,3)</f>
+        <v>Linda</v>
+      </c>
       <c r="D4" s="68"/>
       <c r="F4" s="69"/>
     </row>

</xml_diff>

<commit_message>
Microsoft Excel MATCH() Function
</commit_message>
<xml_diff>
--- a/Section 25: Working with Excel's Lookup Functions/Resources/Excel103-AdvancedExercises.xlsx
+++ b/Section 25: Working with Excel's Lookup Functions/Resources/Excel103-AdvancedExercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolinecrandell/Documents/Employment/*Applications/2022.12 Job Apps/GitHub/excel/Section 25: Working with Excel's Lookup Functions/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C743D1A-2376-5E4B-92A4-325F4919A548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875B52AE-1CB6-B340-AF6F-6F5047C807F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16880" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1964,13 +1964,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2998,10 +2998,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="133" t="s">
+      <c r="E2" s="131" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="133"/>
+      <c r="F2" s="131"/>
     </row>
     <row r="3" spans="2:6" ht="14">
       <c r="B3" s="25" t="s">
@@ -3010,11 +3010,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="131" t="str">
+      <c r="E3" s="132" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="132"/>
+      <c r="F3" s="133"/>
     </row>
     <row r="4" spans="2:6" ht="14">
       <c r="B4" s="25" t="s">
@@ -3023,8 +3023,8 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="131"/>
-      <c r="F4" s="132"/>
+      <c r="E4" s="132"/>
+      <c r="F4" s="133"/>
     </row>
     <row r="5" spans="2:6" ht="14">
       <c r="B5" s="25" t="s">
@@ -3033,8 +3033,8 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="131"/>
-      <c r="F5" s="132"/>
+      <c r="E5" s="132"/>
+      <c r="F5" s="133"/>
     </row>
     <row r="6" spans="2:6" ht="14">
       <c r="B6" s="25" t="s">
@@ -3043,8 +3043,8 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="131"/>
-      <c r="F6" s="132"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="133"/>
     </row>
     <row r="7" spans="2:6" ht="14">
       <c r="B7" s="25" t="s">
@@ -3053,8 +3053,8 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="131"/>
-      <c r="F7" s="132"/>
+      <c r="E7" s="132"/>
+      <c r="F7" s="133"/>
     </row>
     <row r="8" spans="2:6" ht="14">
       <c r="B8" s="25" t="s">
@@ -3063,8 +3063,8 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="131"/>
-      <c r="F8" s="132"/>
+      <c r="E8" s="132"/>
+      <c r="F8" s="133"/>
     </row>
     <row r="9" spans="2:6" ht="14">
       <c r="B9" s="25" t="s">
@@ -3073,8 +3073,8 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="131"/>
-      <c r="F9" s="132"/>
+      <c r="E9" s="132"/>
+      <c r="F9" s="133"/>
     </row>
     <row r="10" spans="2:6" ht="14">
       <c r="B10" s="25" t="s">
@@ -3083,8 +3083,8 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="131"/>
-      <c r="F10" s="132"/>
+      <c r="E10" s="132"/>
+      <c r="F10" s="133"/>
     </row>
     <row r="11" spans="2:6" ht="14">
       <c r="B11" s="25" t="s">
@@ -3093,8 +3093,8 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="131"/>
-      <c r="F11" s="132"/>
+      <c r="E11" s="132"/>
+      <c r="F11" s="133"/>
     </row>
     <row r="12" spans="2:6" ht="14">
       <c r="B12" s="25" t="s">
@@ -3103,8 +3103,8 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="131"/>
-      <c r="F12" s="132"/>
+      <c r="E12" s="132"/>
+      <c r="F12" s="133"/>
     </row>
     <row r="13" spans="2:6" ht="14">
       <c r="B13" s="25" t="s">
@@ -3113,8 +3113,8 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="131"/>
-      <c r="F13" s="132"/>
+      <c r="E13" s="132"/>
+      <c r="F13" s="133"/>
     </row>
     <row r="14" spans="2:6" ht="14">
       <c r="B14" s="25" t="s">
@@ -3123,8 +3123,8 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="131"/>
-      <c r="F14" s="132"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="133"/>
     </row>
     <row r="15" spans="2:6" ht="14">
       <c r="B15" s="25" t="s">
@@ -3133,8 +3133,8 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="131"/>
-      <c r="F15" s="132"/>
+      <c r="E15" s="132"/>
+      <c r="F15" s="133"/>
     </row>
     <row r="16" spans="2:6" ht="14">
       <c r="B16" s="25" t="s">
@@ -3143,8 +3143,8 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="131"/>
-      <c r="F16" s="132"/>
+      <c r="E16" s="132"/>
+      <c r="F16" s="133"/>
     </row>
     <row r="17" spans="2:6" ht="14">
       <c r="B17" s="25" t="s">
@@ -3153,8 +3153,8 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="131"/>
-      <c r="F17" s="132"/>
+      <c r="E17" s="132"/>
+      <c r="F17" s="133"/>
     </row>
     <row r="18" spans="2:6" ht="14">
       <c r="B18" s="25" t="s">
@@ -3163,11 +3163,18 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="131"/>
-      <c r="F18" s="132"/>
+      <c r="E18" s="132"/>
+      <c r="F18" s="133"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3178,13 +3185,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13193,7 +13193,7 @@
   <dimension ref="B2:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -13236,7 +13236,10 @@
         <f>INDEX('INDEX MATCH Master Emp List'!$A$1:$I$38,10,3)</f>
         <v>Linda</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="68">
+        <f>MATCH(B4,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
+        <v>1</v>
+      </c>
       <c r="F4" s="69"/>
     </row>
     <row r="5" spans="2:6">
@@ -13244,7 +13247,10 @@
         <v>1078</v>
       </c>
       <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
+      <c r="D5" s="68">
+        <f>MATCH(B5,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
+        <v>5</v>
+      </c>
       <c r="F5" s="69"/>
     </row>
     <row r="6" spans="2:6">
@@ -13252,7 +13258,10 @@
         <v>1284</v>
       </c>
       <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
+      <c r="D6" s="68">
+        <f>MATCH(B6,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
+        <v>8</v>
+      </c>
       <c r="F6" s="69"/>
     </row>
     <row r="7" spans="2:6">
@@ -13260,7 +13269,10 @@
         <v>1299</v>
       </c>
       <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
+      <c r="D7" s="68">
+        <f>MATCH(B7,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
+        <v>11</v>
+      </c>
       <c r="F7" s="69"/>
     </row>
     <row r="8" spans="2:6">
@@ -13268,7 +13280,10 @@
         <v>1329</v>
       </c>
       <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
+      <c r="D8" s="68">
+        <f>MATCH(B8,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
+        <v>14</v>
+      </c>
       <c r="F8" s="69"/>
     </row>
     <row r="9" spans="2:6">
@@ -13276,7 +13291,10 @@
         <v>1509</v>
       </c>
       <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
+      <c r="D9" s="68">
+        <f>MATCH(B9,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
+        <v>17</v>
+      </c>
       <c r="F9" s="69"/>
     </row>
     <row r="10" spans="2:6">
@@ -13339,7 +13357,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Microsoft Excel INDEX() and MATCH() Function Combined
</commit_message>
<xml_diff>
--- a/Section 25: Working with Excel's Lookup Functions/Resources/Excel103-AdvancedExercises.xlsx
+++ b/Section 25: Working with Excel's Lookup Functions/Resources/Excel103-AdvancedExercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolinecrandell/Documents/Employment/*Applications/2022.12 Job Apps/GitHub/excel/Section 25: Working with Excel's Lookup Functions/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875B52AE-1CB6-B340-AF6F-6F5047C807F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BEF758-724C-8146-8ABF-BCA62E8279AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16880" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13193,7 +13193,7 @@
   <dimension ref="B2:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F4" sqref="F4:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -13240,7 +13240,10 @@
         <f>MATCH(B4,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
         <v>1</v>
       </c>
-      <c r="F4" s="69"/>
+      <c r="F4" s="69" t="str">
+        <f>INDEX('INDEX MATCH Master Emp List'!$D$1:$D$38, MATCH(B4,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
+        <v>AT</v>
+      </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" s="68">
@@ -13251,7 +13254,10 @@
         <f>MATCH(B5,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
         <v>5</v>
       </c>
-      <c r="F5" s="69"/>
+      <c r="F5" s="69" t="str">
+        <f>INDEX('INDEX MATCH Master Emp List'!$D$1:$D$38, MATCH(B5,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
+        <v>AC</v>
+      </c>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="68">
@@ -13262,7 +13268,10 @@
         <f>MATCH(B6,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
         <v>8</v>
       </c>
-      <c r="F6" s="69"/>
+      <c r="F6" s="69" t="str">
+        <f>INDEX('INDEX MATCH Master Emp List'!$D$1:$D$38, MATCH(B6,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
+        <v>MK</v>
+      </c>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="68">
@@ -13273,7 +13282,10 @@
         <f>MATCH(B7,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
         <v>11</v>
       </c>
-      <c r="F7" s="69"/>
+      <c r="F7" s="69" t="str">
+        <f>INDEX('INDEX MATCH Master Emp List'!$D$1:$D$38, MATCH(B7,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
+        <v>MF</v>
+      </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="68">
@@ -13284,7 +13296,10 @@
         <f>MATCH(B8,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
         <v>14</v>
       </c>
-      <c r="F8" s="69"/>
+      <c r="F8" s="69" t="str">
+        <f>INDEX('INDEX MATCH Master Emp List'!$D$1:$D$38, MATCH(B8,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
+        <v>AC</v>
+      </c>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="68">
@@ -13295,7 +13310,10 @@
         <f>MATCH(B9,'INDEX MATCH Master Emp List'!$A$2:$A$38,0)</f>
         <v>17</v>
       </c>
-      <c r="F9" s="69"/>
+      <c r="F9" s="69" t="str">
+        <f>INDEX('INDEX MATCH Master Emp List'!$D$1:$D$38, MATCH(B9,'INDEX MATCH Master Emp List'!$A$1:$A$38,0))</f>
+        <v>AT</v>
+      </c>
     </row>
     <row r="10" spans="2:6">
       <c r="C10" s="68"/>

</xml_diff>

<commit_message>
Creating a Dynamic HLOOKUP() with the MATCH() Function
</commit_message>
<xml_diff>
--- a/Section 25: Working with Excel's Lookup Functions/Resources/Excel103-AdvancedExercises.xlsx
+++ b/Section 25: Working with Excel's Lookup Functions/Resources/Excel103-AdvancedExercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolinecrandell/Documents/Employment/*Applications/2022.12 Job Apps/GitHub/excel/Section 25: Working with Excel's Lookup Functions/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BEF758-724C-8146-8ABF-BCA62E8279AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7EC743-1E2A-A244-AABD-4CF1318D86F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16880" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16940" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -11489,7 +11489,7 @@
   <dimension ref="B1:G18"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C3" sqref="C3:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -11526,19 +11526,19 @@
         <v>1054</v>
       </c>
       <c r="C3" s="11" t="str">
-        <f>IFERROR(VLOOKUP(B3,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B3,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Howard</v>
       </c>
       <c r="D3" s="11" t="str">
-        <f>VLOOKUP($B3, 'Master Emp List'!$A$2:$I$38,2,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B3,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Smith</v>
       </c>
       <c r="E3" s="11" t="str">
-        <f>VLOOKUP($B3, 'Master Emp List'!$A$2:$I$38,4,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B3,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>AT</v>
       </c>
       <c r="F3" s="11">
-        <f>VLOOKUP($B3, 'Master Emp List'!$A$2:$I$38,9,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B3,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>11.25</v>
       </c>
       <c r="G3" s="67"/>
@@ -11548,19 +11548,19 @@
         <v>1056</v>
       </c>
       <c r="C4" s="11" t="str">
-        <f>IFERROR(VLOOKUP(B4,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B4,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Joe</v>
       </c>
       <c r="D4" s="11" t="str">
-        <f>VLOOKUP($B4, 'Master Emp List'!$A$2:$I$38,2,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B4,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Gonzales</v>
       </c>
       <c r="E4" s="11" t="str">
-        <f>VLOOKUP($B4, 'Master Emp List'!$A$2:$I$38,4,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B4,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>AT</v>
       </c>
       <c r="F4" s="11">
-        <f>VLOOKUP($B4, 'Master Emp List'!$A$2:$I$38,9,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B4,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>12.25</v>
       </c>
       <c r="G4" s="67"/>
@@ -11570,19 +11570,19 @@
         <v>1067</v>
       </c>
       <c r="C5" s="11" t="str">
-        <f>IFERROR(VLOOKUP(B5,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B5,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Gail</v>
       </c>
       <c r="D5" s="11" t="str">
-        <f>VLOOKUP($B5, 'Master Emp List'!$A$2:$I$38,2,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B5,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Scote</v>
       </c>
       <c r="E5" s="11" t="str">
-        <f>VLOOKUP($B5, 'Master Emp List'!$A$2:$I$38,4,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B5,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>AT</v>
       </c>
       <c r="F5" s="11">
-        <f>VLOOKUP($B5, 'Master Emp List'!$A$2:$I$38,9,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B5,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>14.55</v>
       </c>
       <c r="G5" s="67"/>
@@ -11592,19 +11592,19 @@
         <v>1075</v>
       </c>
       <c r="C6" s="11" t="str">
-        <f>IFERROR(VLOOKUP(B6,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B6,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Sheryl</v>
       </c>
       <c r="D6" s="11" t="str">
-        <f>VLOOKUP($B6, 'Master Emp List'!$A$2:$I$38,2,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B6,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Kane</v>
       </c>
       <c r="E6" s="11" t="str">
-        <f>VLOOKUP($B6, 'Master Emp List'!$A$2:$I$38,4,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B6,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>AD</v>
       </c>
       <c r="F6" s="11">
-        <f>VLOOKUP($B6, 'Master Emp List'!$A$2:$I$38,9,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B6,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>11.25</v>
       </c>
       <c r="G6" s="67"/>
@@ -11614,19 +11614,19 @@
         <v>1078</v>
       </c>
       <c r="C7" s="11" t="str">
-        <f>IFERROR(VLOOKUP(B7,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B7,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Kendrick</v>
       </c>
       <c r="D7" s="11" t="str">
-        <f>VLOOKUP($B7, 'Master Emp List'!$A$2:$I$38,2,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B7,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Hapsbuch</v>
       </c>
       <c r="E7" s="11" t="str">
-        <f>VLOOKUP($B7, 'Master Emp List'!$A$2:$I$38,4,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B7,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>AC</v>
       </c>
       <c r="F7" s="11">
-        <f>VLOOKUP($B7, 'Master Emp List'!$A$2:$I$38,9,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B7,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>10.199999999999999</v>
       </c>
       <c r="G7" s="67"/>
@@ -11636,19 +11636,19 @@
         <v>1152</v>
       </c>
       <c r="C8" s="11" t="str">
-        <f>IFERROR(VLOOKUP(B8,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B8,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Mark</v>
       </c>
       <c r="D8" s="11" t="str">
-        <f>VLOOKUP($B8, 'Master Emp List'!$A$2:$I$38,2,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B8,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Henders</v>
       </c>
       <c r="E8" s="11" t="str">
-        <f>VLOOKUP($B8, 'Master Emp List'!$A$2:$I$38,4,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B8,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>AD</v>
       </c>
       <c r="F8" s="11">
-        <f>VLOOKUP($B8, 'Master Emp List'!$A$2:$I$38,9,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B8,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>12.25</v>
       </c>
       <c r="G8" s="67"/>
@@ -11658,19 +11658,19 @@
         <v>1196</v>
       </c>
       <c r="C9" s="11" t="str">
-        <f>IFERROR(VLOOKUP(B9,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B9,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Katie</v>
       </c>
       <c r="D9" s="11" t="str">
-        <f>VLOOKUP($B9, 'Master Emp List'!$A$2:$I$38,2,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B9,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Atherton</v>
       </c>
       <c r="E9" s="11" t="str">
-        <f>VLOOKUP($B9, 'Master Emp List'!$A$2:$I$38,4,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B9,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>HR</v>
       </c>
       <c r="F9" s="11">
-        <f>VLOOKUP($B9, 'Master Emp List'!$A$2:$I$38,9,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B9,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>9.9499999999999993</v>
       </c>
       <c r="G9" s="67"/>
@@ -11680,19 +11680,19 @@
         <v>1284</v>
       </c>
       <c r="C10" s="11" t="str">
-        <f>IFERROR(VLOOKUP(B10,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B10,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Frank</v>
       </c>
       <c r="D10" s="11" t="str">
-        <f>VLOOKUP($B10, 'Master Emp List'!$A$2:$I$38,2,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B10,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Bellwood</v>
       </c>
       <c r="E10" s="11" t="str">
-        <f>VLOOKUP($B10, 'Master Emp List'!$A$2:$I$38,4,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B10,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>MK</v>
       </c>
       <c r="F10" s="11">
-        <f>VLOOKUP($B10, 'Master Emp List'!$A$2:$I$38,9,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B10,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>12.3</v>
       </c>
       <c r="G10" s="67"/>
@@ -11701,60 +11701,60 @@
       <c r="B11" s="10">
         <v>100</v>
       </c>
-      <c r="C11" s="11" t="str">
-        <f>IFERROR(VLOOKUP(B11,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
-        <v>EMP ID NOT FOUND</v>
+      <c r="C11" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B11,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
       </c>
       <c r="D11" s="11" t="e">
-        <f>VLOOKUP($B11, 'Master Emp List'!$A$2:$I$38,2,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B11,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>#N/A</v>
       </c>
       <c r="E11" s="11" t="e">
-        <f>VLOOKUP($B11, 'Master Emp List'!$A$2:$I$38,4,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B11,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>#N/A</v>
       </c>
       <c r="F11" s="11" t="e">
-        <f>VLOOKUP($B11, 'Master Emp List'!$A$2:$I$38,9,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B11,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>#N/A</v>
       </c>
       <c r="G11" s="67"/>
     </row>
     <row r="12" spans="2:7">
       <c r="B12" s="10"/>
-      <c r="C12" s="11" t="str">
-        <f>IFERROR(VLOOKUP(B12,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
-        <v>EMP ID NOT FOUND</v>
+      <c r="C12" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B12,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
       </c>
       <c r="D12" s="11" t="e">
-        <f>VLOOKUP($B12, 'Master Emp List'!$A$2:$I$38,2,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B12,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>#N/A</v>
       </c>
       <c r="E12" s="11" t="e">
-        <f>VLOOKUP($B12, 'Master Emp List'!$A$2:$I$38,4,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B12,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>#N/A</v>
       </c>
       <c r="F12" s="11" t="e">
-        <f>VLOOKUP($B12, 'Master Emp List'!$A$2:$I$38,9,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B12,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>#N/A</v>
       </c>
       <c r="G12" s="67"/>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="10"/>
-      <c r="C13" s="11" t="str">
-        <f>IFERROR(VLOOKUP(B13,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
-        <v>EMP ID NOT FOUND</v>
+      <c r="C13" s="11" t="e">
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B13,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
+        <v>#N/A</v>
       </c>
       <c r="D13" s="11" t="e">
-        <f>VLOOKUP($B13, 'Master Emp List'!$A$2:$I$38,2,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B13,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>#N/A</v>
       </c>
       <c r="E13" s="11" t="e">
-        <f>VLOOKUP($B13, 'Master Emp List'!$A$2:$I$38,4,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B13,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>#N/A</v>
       </c>
       <c r="F13" s="11" t="e">
-        <f>VLOOKUP($B13, 'Master Emp List'!$A$2:$I$38,9,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B13,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>#N/A</v>
       </c>
       <c r="G13" s="67"/>
@@ -11764,19 +11764,19 @@
         <v>1302</v>
       </c>
       <c r="C14" s="11" t="str">
-        <f>IFERROR(VLOOKUP(B14,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B14,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Randy</v>
       </c>
       <c r="D14" s="11" t="str">
-        <f>VLOOKUP($B14, 'Master Emp List'!$A$2:$I$38,2,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B14,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Sindole</v>
       </c>
       <c r="E14" s="11" t="str">
-        <f>VLOOKUP($B14, 'Master Emp List'!$A$2:$I$38,4,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B14,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>MK</v>
       </c>
       <c r="F14" s="11">
-        <f>VLOOKUP($B14, 'Master Emp List'!$A$2:$I$38,9,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B14,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>14.25</v>
       </c>
       <c r="G14" s="67"/>
@@ -11786,19 +11786,19 @@
         <v>1310</v>
       </c>
       <c r="C15" s="11" t="str">
-        <f>IFERROR(VLOOKUP(B15,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B15,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Ellen</v>
       </c>
       <c r="D15" s="11" t="str">
-        <f>VLOOKUP($B15, 'Master Emp List'!$A$2:$I$38,2,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B15,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Smith</v>
       </c>
       <c r="E15" s="11" t="str">
-        <f>VLOOKUP($B15, 'Master Emp List'!$A$2:$I$38,4,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B15,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>MF</v>
       </c>
       <c r="F15" s="11">
-        <f>VLOOKUP($B15, 'Master Emp List'!$A$2:$I$38,9,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B15,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>11.5</v>
       </c>
       <c r="G15" s="67"/>
@@ -11808,19 +11808,19 @@
         <v>1329</v>
       </c>
       <c r="C16" s="11" t="str">
-        <f>IFERROR(VLOOKUP(B16,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B16,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Tuome</v>
       </c>
       <c r="D16" s="11" t="str">
-        <f>VLOOKUP($B16, 'Master Emp List'!$A$2:$I$38,2,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B16,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Vuanuo</v>
       </c>
       <c r="E16" s="11" t="str">
-        <f>VLOOKUP($B16, 'Master Emp List'!$A$2:$I$38,4,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B16,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>AC</v>
       </c>
       <c r="F16" s="11">
-        <f>VLOOKUP($B16, 'Master Emp List'!$A$2:$I$38,9,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B16,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>10.35</v>
       </c>
       <c r="G16" s="67"/>
@@ -11830,19 +11830,19 @@
         <v>1333</v>
       </c>
       <c r="C17" s="11" t="str">
-        <f>IFERROR(VLOOKUP(B17,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B17,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Tadeuz</v>
       </c>
       <c r="D17" s="11" t="str">
-        <f>VLOOKUP($B17, 'Master Emp List'!$A$2:$I$38,2,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B17,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Szcznyck</v>
       </c>
       <c r="E17" s="11" t="str">
-        <f>VLOOKUP($B17, 'Master Emp List'!$A$2:$I$38,4,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B17,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>HR</v>
       </c>
       <c r="F17" s="11">
-        <f>VLOOKUP($B17, 'Master Emp List'!$A$2:$I$38,9,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B17,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>10.15</v>
       </c>
       <c r="G17" s="67"/>
@@ -11852,19 +11852,19 @@
         <v>1368</v>
       </c>
       <c r="C18" s="11" t="str">
-        <f>IFERROR(VLOOKUP(B18,'Master Emp List'!$A$1:$I$38,3,FALSE), "EMP ID NOT FOUND")</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B18,'Master Emp List'!$A$1:$A$38,0),MATCH(C$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Tammy</v>
       </c>
       <c r="D18" s="11" t="str">
-        <f>VLOOKUP($B18, 'Master Emp List'!$A$2:$I$38,2,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B18,'Master Emp List'!$A$1:$A$38,0),MATCH(D$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>Wu</v>
       </c>
       <c r="E18" s="11" t="str">
-        <f>VLOOKUP($B18, 'Master Emp List'!$A$2:$I$38,4,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B18,'Master Emp List'!$A$1:$A$38,0),MATCH(E$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>AD</v>
       </c>
       <c r="F18" s="11">
-        <f>VLOOKUP($B18, 'Master Emp List'!$A$2:$I$38,9,FALSE)</f>
+        <f>INDEX('Master Emp List'!$A$1:$I$38, MATCH($B18,'Master Emp List'!$A$1:$A$38,0),MATCH(F$2,'Master Emp List'!$A$1:$I$1,0))</f>
         <v>12.25</v>
       </c>
       <c r="G18" s="67"/>
@@ -13004,8 +13004,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -13044,7 +13044,7 @@
         <v>229</v>
       </c>
       <c r="B5" s="57">
-        <f>HLOOKUP($B$3,'Master Inventory List'!$A$2:$G$5,2,FALSE)</f>
+        <f>HLOOKUP($B$3,'Master Inventory List'!$A$2:$G$5,MATCH(LEFT(A5,11),'Master Inventory List'!$A$2:$A$5,0),FALSE)</f>
         <v>150</v>
       </c>
     </row>
@@ -13053,7 +13053,7 @@
         <v>228</v>
       </c>
       <c r="B6" s="57">
-        <f>HLOOKUP($B$3,'Master Inventory List'!$A$2:$G$5,3,FALSE)</f>
+        <f>HLOOKUP($B$3,'Master Inventory List'!$A$2:$G$5,MATCH(LEFT(A6,11),'Master Inventory List'!$A$2:$A$5,0),FALSE)</f>
         <v>110</v>
       </c>
     </row>
@@ -13062,7 +13062,7 @@
         <v>227</v>
       </c>
       <c r="B7" s="57">
-        <f>HLOOKUP($B$3,'Master Inventory List'!$A$2:$G$5,4,FALSE)</f>
+        <f>HLOOKUP($B$3,'Master Inventory List'!$A$2:$G$5,MATCH(LEFT(A7,11),'Master Inventory List'!$A$2:$A$5,0),FALSE)</f>
         <v>115</v>
       </c>
     </row>
@@ -13192,7 +13192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A99380-3415-42C6-8C41-613698A280FA}">
   <dimension ref="B2:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F4" sqref="F4:F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>